<commit_message>
added 100 more judgements refined
</commit_message>
<xml_diff>
--- a/web_scraper/processed_judgements_final/2023LHC7518.xlsx
+++ b/web_scraper/processed_judgements_final/2023LHC7518.xlsx
@@ -453,17 +453,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> * On May 29, 2013, the dead body of an unknown woman was found in a field near Chak No. 305/TDA, Tehsil Karor. * The police registered a case (FIR No. 207/2013) against Muhammad Nadeem and Yasir Ali under sections 302 and 34 PPC. * The prosecution alleged that the accused had murdered the woman, Momna Bibi alias Saba, due to her immoral activities and her refusal to obey her husband's (accused Nadeem's) orders. * The prosecution claimed that Nadeem and Yasir Ali had committed the murder with the help of a motorcycle, and that Nadeem had confessed to the crime during an extrajudicial confession.  The crime scenario involves the murder of a woman, Momna Bibi alias Saba, who was found dead with severe injuries near a canal. The investigation led to the arrest of the appellant, Muhammad Nadeem, and his co-accused, Yasir Ali. The prosecution alleged that the appellant and Yasir Ali threw the baby of Momna Bibi into the canal and then murdered her. The prosecution relied on the testimony of several witnesses, including foot trackers, who identified the appellant's footprints at the scene of the crime.   The appellant, Muhammad Nadeem, was charged with the murder of his wife, Momna Bibi alias Saba (deceased). The prosecution alleged that the appellant and his co-accused, Yasir Ali (since acquitted), committed the murder due to a motive stemming from the fact that Momna Bibi alias Saba had contracted a second marriage with the appellant without the consent of her parents, Mst. Bachal Mai and others. The prosecution also alleged that the appellant recovered a Churri (a type of cloth) and a motorcycle from his residence, which were linked to the crime.  </t>
+          <t xml:space="preserve">Muhammad Nadeem, the appellant, was accused of murdering Momna Bibi alias Saba on May 29, 2013. The prosecution alleged that Nadeem had murdered Saba due to her immoral activities and her decision to go to D.G. Khan to visit her mother despite his objections. The prosecution's case was based on circumstantial evidence, including the testimony of witnesses who claimed to have seen Nadeem at the scene of the crime, footprints and tire marks found at the scene, and a confession allegedly made by Nadeem to two witnesses. The prosecution also produced medical evidence, including a post-mortem report, and a report from the Punjab Forensic Science Agency.   * The appellant, Muhammad Nadeem, was accused of murdering his cousin's wife, Momna Bibi alias Saba, and throwing her baby into a canal. * The prosecution alleged that the appellant was seen with Yasir Ali, another accused, on the night of the murder, and that they threw the baby into the canal. * The prosecution relied on the testimony of several witnesses, including a foot tracker, Muhammad Iqbal, who identified the appellant's footprints at the scene of the crime.   The appellant, Muhammad Nadeem, was accused of murdering his wife, Momna Bibi alias Saba, along with his co-accused Yasir Ali. The motive for the murder was allegedly due to the strained relations between the spouses, as Momna Bibi had contracted a second marriage without the appellant's consent. The prosecution's evidence included the recovery of a Churri (a type of cloth) and a motorcycle, as well as the testimony of Mst. Bachal Mai, who claimed that Momna Bibi had married the appellant against their wishes. However, the prosecution failed to provide substantial evidence to prove the motive, and the recovery of the Churri and motorcycle was deemed inconsequential.  </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> * 16 prosecution witnesses testified during the trial, including: 	+ Muhammad Nasrullah, ASI (PW.1), who kept the evidence in the police station. 	+ Muhammad Younis, recovery witness (PW.2), who recovered the moulds of the accused's footprints and the motorcycle's tyres. 	+ Mansab Ali Patwari (PW.3), who prepared scaled site plans of the place of occurrence. 	+ Rashid Imran and Tahir Saleem alias Tariq Saleem (PW.8 and PW.9), who allegedly witnessed the extrajudicial confession of Nadeem. 	+ Muhammad Iqbal, foot tracker (PW.11), who prepared the moulds of the accused's footprints and the motorcycle's tyres. 	+ Other witnesses, including the mother of the deceased, Mst. Bachal Mai (PW.10), and the investigating officers, Zafar Iqbal and Ghulam Qadir (PW.13 and PW.15).  The witnesses who testified on behalf of the prosecution included:  * Muhammad Iqbal, the foot tracker, who prepared moulds of footprints and identified the appellant's footprints at the scene of the crime. * Muhammad Anwar, the recovery witness, who recovered the moulds of a male and tyres of a motorcycle from the scene of the crime. * Lady Doctor Kausar Parveen, who conducted the autopsy on the dead body of Momna Bibi. * Mst. Bachal Mai, the mother of Momina Bibi, who identified her daughter's body. * Muhammad Numan and Sana Ullah, who claimed to have seen the appellant and Yasir Ali throwing the baby into the canal.   * Mst. Bachal Mai (PW.10) testified that Momna Bibi alias Saba had contracted a second marriage with the appellant without their consent, but she could not produce any documents or witnesses to support her claim. * Ghulam Qadir SI/I.O (PW.15) testified that Mst. Bachal Mai orally stated that Momna Bibi alias Saba had contracted a second marriage with the appellant against their wishes, but she could not produce any documents or witnesses to support her claim.  </t>
+          <t xml:space="preserve">The prosecution produced 16 witnesses, including:  * Muhammad Nasrullah, an ASI who recovered various items from the crime scene * Muhammad Younis, a recovery witness who testified about the recovery of moulds of Nadeem's footprints and tires of a motorcycle * Mansab Ali Patwari, who prepared scaled site plans of the crime scene * Rashid Imran and Tahir Saleem, who testified about the alleged extrajudicial confession made by Nadeem * Muhammad Iqbal, a foot tracker who prepared moulds of Nadeem's footprints and tires of a motorcycle * Mst. Bachal Mai, the mother of the deceased, who identified the body and nominated Nadeem as the killer * Zafar Iqbal and Ghulam Qadir, the investigating officers who testified about the investigation and recovery of evidence   * Muhammad Iqbal (PW.11), the foot tracker, identified the appellant's footprints at the scene of the crime, but his evidence was criticized for being weak and unreliable. * Muhammad Anwar (PW.12), the recovery witness, testified that he found the appellant's moulds of footprints and motorcycle tyres at the scene of the crime. * Mst. Bachal Mai (PW.10), the mother of the deceased, testified that her daughter was 17-18 years old at the time of her death, which contradicted the prosecution's claim that the deceased was 35 years old. * Muhammad Numan (PW.14) and Sana Ullah (PW.16) testified that they saw the appellant and Yasir Ali throwing the baby into the canal, but their evidence was criticized for being unreliable and uncorroborated.   * Mst. Bachal Mai (PW.10) testified that Momna Bibi had married the appellant against their wishes, but could not produce any documents or witnesses to support this claim. * Ghulam Qadir SI/I.O (PW.15) testified that Mst. Bachal Mai orally stated that Momna Bibi had married the appellant against their wishes, but could not provide any evidence to support this claim.  </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> * The trial court convicted Nadeem of the murder and sentenced him to life imprisonment, with a fine of Rs. 2,00,000 to the legal heirs of the deceased. * The appeal court has acquitted Nadeem of the charge, holding that the evidence of extrajudicial confession is fabricated and does not bear any credibility. * The court also held that the evidence of foot tracking and the report of the Punjab Forensic Science Agency are weak and do not provide sufficient evidence to connect Nadeem to the crime. * The court relied on the Supreme Court judgments in "Hashim Qasim and another v. The State", "Fayyaz Ahmad v. The State", and "Sadi Ahmad and another v. The State" to hold that the prosecution has failed to prove its case beyond any shadow of doubt. The court found that the prosecution's evidence was not reliable and did not raise a high degree of probability of the appellant's guilt. The court specifically found that:  * The foot tracker's evidence was weak and did not meet the requirements of Rule 26 of the Punjab Police Rules, 1934. * The recovery witness's evidence was not reliable, as he failed to justify his presence at the scene of the crime. * The medical evidence, while confirming the receipt of injuries, did not identify the assailant. * The testimony of Muhammad Numan and Sana Ullah was not credible, as they failed to justify their presence at the scene of the crime and their conduct was unnatural. * The acquittal of Yasir Ali, the co-accused, meant that the prosecution's witnesses were not reliable with respect to the other co-accused, unless supported by corroboratory evidence from an independent source.  **Verdict and Sentencing:** The court acquitted the appellant, Muhammad Nadeem, of the charges of murder and throwing the baby into the canal.  **Basis of Decision:** The court's decision was based on the lack of reliable evidence and the weaknesses in the prosecution's case. The court applied the principles of law and justice, including the requirement for corroboratory evidence from an independent source and the need for a high degree of probability of guilt.  The court acquitted the appellant, Muhammad Nadeem, of the charge of murder due to the lack of substantial evidence to prove the motive. The court held that the prosecution failed to establish the motive part of the occurrence, and the only evidence remaining was the oral assertion of Mst. Bachal Mai, which was not sufficient to prove the guilt of the appellant. The court also relied on the principles of criminal jurisprudence that if the prosecution sets up a motive but fails to prove it, then it is the prosecution who has to suffer and not the accused. The court further held that the case against the appellant was replete with doubts, and the benefit of doubt should be given to the accused as a matter of right. </t>
+          <t xml:space="preserve">The learned trial court convicted Nadeem of murder and sentenced him to life imprisonment. The trial court acquitted his co-accused, Yasir Ali, due to lack of evidence.  The High Court, however, has set aside the conviction and acquitted Nadeem due to lack of credible evidence. The court held that the evidence of extrajudicial confession was fabricated and did not bear any credibility. The court also noted that the prosecution's case was based on circumstantial evidence, which was not sufficient to prove Nadeem's guilt beyond a reasonable doubt. The court relied on Supreme Court judgments that declared extrajudicial confession as a weak type of evidence.  * The court found that the prosecution's evidence was weak and unreliable, and that the foot tracker's evidence was particularly unreliable. * The court noted that the prosecution failed to prove safe custody of the moulds of footprints and motorcycle tyres, and that the foot tracker did not follow the proper procedure for preparing and preserving the moulds. * The court also criticized the testimony of Muhammad Numan (PW.14) and Sana Ullah (PW.16) as unreliable and uncorroborated. * The court concluded that the prosecution failed to prove the appellant's guilt beyond a reasonable doubt, and accordingly acquitted the appellant of the charge.  The Supreme Court of Pakistan acquitted the appellant, Muhammad Nadeem, of the charge of murder due to the lack of substantial evidence to prove the motive and the inconsequential nature of the recovery of the Churri and motorcycle. The Court held that in the event of a doubt, the benefit must be given to the accused, and that the prosecution had failed to establish the motive part of the occurrence. The appellant was ordered to be released forthwith if not required in any other case. </t>
         </is>
       </c>
     </row>

</xml_diff>